<commit_message>
BERTScore and human_evaluations added to repo.
</commit_message>
<xml_diff>
--- a/experiments/roberta/results/five_answer_best_context_concat.xlsx
+++ b/experiments/roberta/results/five_answer_best_context_concat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhysb\Git_Repositories\iTA\experiments\roberta\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B19489-4B5D-4609-8B12-093A9E30D6CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA979F6-BBFD-40D4-B779-1820B5E8D315}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2236,8 +2236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView tabSelected="1" topLeftCell="D116" workbookViewId="0">
+      <selection activeCell="J116" sqref="J116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4102,7 +4102,7 @@
         <v>53.7307017976213</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="360" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="345" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>239</v>
       </c>

</xml_diff>